<commit_message>
changes to linkes in job application project
</commit_message>
<xml_diff>
--- a/JobApplicaiton/link.xlsx
+++ b/JobApplicaiton/link.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahith\Desktop\All-code\PersonalAutomations\JobApplicaiton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFF64F5-24D0-45AF-AA6C-094CFD4D44D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EB8E7B-34BA-4C1C-8166-8044E53A94BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tech" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="143">
   <si>
     <t>Facebook</t>
   </si>
@@ -143,9 +143,6 @@
     <t>https://jobs.sutterhealth.org/us/en/c/information-services-jobs</t>
   </si>
   <si>
-    <t>sutter health</t>
-  </si>
-  <si>
     <t>https://www.disneycareers.com/en/search-jobs?k=software&amp;l=&amp;orgIds=391</t>
   </si>
   <si>
@@ -156,6 +153,312 @@
   </si>
   <si>
     <t>https://jobs.ea.com/en_US/careers/Home/?8171=%5B10618%5D&amp;8171_format=5683&amp;4536=%5B8306%2C8301%2C8331%2C8321%2C257281%5D&amp;4536_format=3019&amp;4537=%5B8695%2C8691%5D&amp;4537_format=3020&amp;listFilterMode=1&amp;jobSort=schemaField_3_136_3&amp;jobSortDirection=DESC&amp;jobRecordsPerPage=20&amp;</t>
+  </si>
+  <si>
+    <t>Crowd Strike</t>
+  </si>
+  <si>
+    <t>https://crowdstrike.wd5.myworkdayjobs.com/en-US/crowdstrikecareers?Job_Family=1408861ee6e20197f95adbf6b000d20b&amp;Job_Family=cb19f044639b1001f6a02595bc920000&amp;Job_Family=1408861ee6e201641be2c2f6b000c00b&amp;workerSubType=f79adfd173da0111b8abd137e373b310&amp;shared_id=MzZkNDhiZTktN2Q4My00MDRlLThkNGMtNTY0ZTBlNmJhMzMz&amp;locationCountry=bc33aa3152ec42d4995f4791a106ed09</t>
+  </si>
+  <si>
+    <t>Reddit</t>
+  </si>
+  <si>
+    <t>https://redditinc.com/careers#</t>
+  </si>
+  <si>
+    <t>https://redhat.wd5.myworkdayjobs.com/jobs/?q=full%20stack&amp;a=bc33aa3152ec42d4995f4791a106ed09</t>
+  </si>
+  <si>
+    <t>Red hat</t>
+  </si>
+  <si>
+    <t>Dimunetional fund advisers</t>
+  </si>
+  <si>
+    <t>https://dimensional.wd5.myworkdayjobs.com/DFA_Careers</t>
+  </si>
+  <si>
+    <t>PNC</t>
+  </si>
+  <si>
+    <t>https://careers.pnc.com/global/en/c/technology-jobs#ph-YTMET</t>
+  </si>
+  <si>
+    <t>Bank of America</t>
+  </si>
+  <si>
+    <t>https://careers.bankofamerica.com/en-us/job-search?ref=search&amp;start=0&amp;rows=10&amp;search=jobsByLocation&amp;filters=area%3DTechnology&amp;sort=newest&amp;searchstring=United+States#</t>
+  </si>
+  <si>
+    <t>Wells fargo</t>
+  </si>
+  <si>
+    <t>https://www.wellsfargojobs.com/en/jobs/?country=United+States+of+America&amp;team=Data+%26+Analytics&amp;team=Investments+%26+Trading&amp;team=Technology+%26+Data&amp;pagesize=20#results</t>
+  </si>
+  <si>
+    <t>https://raymondjames.wd1.myworkdayjobs.com/RaymondJamesCareers?q=software&amp;Country=bc33aa3152ec42d4995f4791a106ed09</t>
+  </si>
+  <si>
+    <t>Raymond James</t>
+  </si>
+  <si>
+    <t>IBM</t>
+  </si>
+  <si>
+    <t>https://www.ibm.com/careers/search?field_keyword_08[0]=Software%20Engineering&amp;field_keyword_08[1]=Infrastructure%20%26%20Technology&amp;field_keyword_08[2]=Data%20%26%20Analytics&amp;field_keyword_18[0]=Entry%20Level&amp;field_keyword_05[0]=United%20States</t>
+  </si>
+  <si>
+    <t>https://careers.toasttab.com/jobs/search?page=1&amp;department_uids%5B%5D=bd322ae656d94bc9bbf37eed696b4add&amp;department_uids%5B%5D=546da8e254b79111ee592914ea196336&amp;department_uids%5B%5D=6183f48dcc6321987e49d5452d208a0d&amp;department_uids%5B%5D=035c08c344393a2d9a7fdcdd5f45896a&amp;country_codes%5B%5D=US&amp;query=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toast </t>
+  </si>
+  <si>
+    <t>CSV</t>
+  </si>
+  <si>
+    <t>https://jobs.cvshealth.com/us/en/search-results</t>
+  </si>
+  <si>
+    <t>shutter health</t>
+  </si>
+  <si>
+    <t>https://gusto.com/about/careers/join-the-team</t>
+  </si>
+  <si>
+    <t>Gusto</t>
+  </si>
+  <si>
+    <t>Onepay</t>
+  </si>
+  <si>
+    <t>https://jobs.ashbyhq.com/oneapp</t>
+  </si>
+  <si>
+    <t>Infosis</t>
+  </si>
+  <si>
+    <t>https://digitalcareers.infosys.com/infosys/global-careers?location=USA</t>
+  </si>
+  <si>
+    <t>https://careers.rivian.com/careers-home/jobs?keywords=software&amp;locations=Atlanta,Georgia,United%20States%7CAustin,Texas,United%20States%7CBlauvelt,New%20York,United%20States%7CCarson,California,United%20States%7CChelsea,Massachusetts,United%20States%7CChicago,Illinois,United%20States%7CDallas,Texas,United%20States%7CDenver,Colorado,United%20States%7CEl%20Segundo,California,United%20States%7CHouston,Texas,United%20States%7CIrvine,California,United%20States%7CMadison%20Heights,Michigan,United%20States%7CMalvern,Pennsylvania,United%20States%7CMcLean,Virginia,United%20States%7CMiami,Florida,United%20States%7CNormal,Illinois,United%20States%7COlathe,Kansas,United%20States%7COrlando,Florida,United%20States%7CPalo%20Alto,California,United%20States%7CPlymouth,Michigan,United%20States%7CRichmond,British%20Columbia,Canada%7CRichmond,Virginia,United%20States%7CSalt%20Lake%20City,Utah,United%20States%7CSan%20Jose,California,United%20States%7CShepherdsville,Kentucky,United%20States%7CSocial%20Circle,Georgia,United%20States%7CSouthhampton,New%20York,United%20States%7CTorrance,California,United%20States%7CTustin,California,United%20States%7CWashington%20D.C.,Washington,United%20States%7CWashington,Washington~%20DC,United%20States%7CWittmann,Arizona,United%20States&amp;page=1&amp;categories=Autonomous%20Driving%7CInformation%20Technology%7CQuality%7CSoftware%20Engineering%7CTest%20and%20Development&amp;sortBy=posted_date&amp;descending=true</t>
+  </si>
+  <si>
+    <t>Rivian</t>
+  </si>
+  <si>
+    <t>Lambda</t>
+  </si>
+  <si>
+    <t>https://lambda.ai/careers#join</t>
+  </si>
+  <si>
+    <t>https://jobs.cisco.com/jobs/SearchJobs/?21178=%5B169482%5D&amp;21178_format=6020&amp;21180=%5B162%2C163%2C164%2C166%5D&amp;21180_format=6022&amp;21181=%5B194%2C187%2C191%2C197%2C55816092%5D&amp;21181_format=6023&amp;listFilterMode=1</t>
+  </si>
+  <si>
+    <t>cisco</t>
+  </si>
+  <si>
+    <t>Kraken</t>
+  </si>
+  <si>
+    <t>https://jobs.ashbyhq.com/kraken.com?departmentId=5f67bd79-103b-4ac1-8d79-952b45ea47c9&amp;locationId=a80c78e5-2d6d-4da1-9f7d-b77def8f4f03</t>
+  </si>
+  <si>
+    <t>Cars commers</t>
+  </si>
+  <si>
+    <t>https://cars.wd12.myworkdayjobs.com/cars?q=software&amp;locations=cb49c6c65b17100131b4de3cdc440000&amp;locations=c4b2ef5945ee100131b48674073e0000</t>
+  </si>
+  <si>
+    <t>Upstart</t>
+  </si>
+  <si>
+    <t>https://careers.upstart.com/jobs/search?page=1&amp;category_uids%5B%5D=f6b0b8a1865c709cf148fc22ecf1d8e7&amp;query=</t>
+  </si>
+  <si>
+    <t>Realter.com</t>
+  </si>
+  <si>
+    <t>https://careers.realtor.com/job-search-results/?keyword=software&amp;primary_category[]=Data%20Science%20and%20Analytics&amp;primary_category[]=Technology</t>
+  </si>
+  <si>
+    <t>https://www.myrocketcareer.com/careers/?search=software&amp;mylocation=United+States&amp;team=Data&amp;team=Technology&amp;team=Finance&amp;pagesize=20&amp;locname=&amp;lat=38.7945952&amp;lng=-106.5348379#results</t>
+  </si>
+  <si>
+    <t>Rocket company careers</t>
+  </si>
+  <si>
+    <t>Charls Shwab</t>
+  </si>
+  <si>
+    <t>https://www.schwabjobs.com/search-jobs</t>
+  </si>
+  <si>
+    <t>https://zillow.wd5.myworkdayjobs.com/Zillow_Group_External?q=software&amp;locations=bf3166a9227a01f8b514f0b00b147bc9</t>
+  </si>
+  <si>
+    <t>Zillo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>https://www.quantiqpartners.com/full-time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantiqparetners </t>
+  </si>
+  <si>
+    <t>digital Oceans</t>
+  </si>
+  <si>
+    <t>https://www.digitalocean.com/careers/open-roles</t>
+  </si>
+  <si>
+    <t>https://www.atlassian.com/company/careers/all-jobs?team=Data%2C%20Analytics%20%26%20Research%2CEngineering%2CSite%20Reliability%20Engineering%2CAtlassian%20Corporate%20Engineering%20%28ACE%29%2CGraduates&amp;location=United%20States&amp;search=</t>
+  </si>
+  <si>
+    <t>Atlassian</t>
+  </si>
+  <si>
+    <t>Geenral Motors</t>
+  </si>
+  <si>
+    <t>https://search-careers.gm.com/en/jobs/?search=software&amp;country=United+States+of+America&amp;team=Data+Management+%26+Analytics&amp;team=Engineering&amp;team=Information+Technology&amp;team=Software+and+Services+Group&amp;team=Students+%26+Recent+Graduates&amp;pagesize=20#results</t>
+  </si>
+  <si>
+    <t>Confluent</t>
+  </si>
+  <si>
+    <t>https://careers.confluent.io/open-positions/early_talent-engineering-united_states</t>
+  </si>
+  <si>
+    <t>Bumble</t>
+  </si>
+  <si>
+    <t>Invisibles.Ai</t>
+  </si>
+  <si>
+    <t>Applied Materials</t>
+  </si>
+  <si>
+    <t>Ebay</t>
+  </si>
+  <si>
+    <t>Hubstaf</t>
+  </si>
+  <si>
+    <t>sailpoint</t>
+  </si>
+  <si>
+    <t>HEB</t>
+  </si>
+  <si>
+    <t>https://jobs.lever.co/bumbleinc</t>
+  </si>
+  <si>
+    <t>https://www.invisible.ai/careers</t>
+  </si>
+  <si>
+    <t>https://careers.appliedmaterials.com/careers?query=software&amp;location=any&amp;Country=United%20States%20of%20America&amp;domain=appliedmaterials.com&amp;sort_by=relevance&amp;pid=790304053974</t>
+  </si>
+  <si>
+    <t>https://jobs.ebayinc.com/us/en/c/engineering-jobs?from=20&amp;s=1</t>
+  </si>
+  <si>
+    <t>https://hubstaff.com/jobs#hsds-open-positions</t>
+  </si>
+  <si>
+    <t>https://sailpoint.wd1.myworkdayjobs.com/SailPoint/jobs?q=python&amp;jobFamilyGroup=b0d5a0c394c810a2b2b41b6251e64819&amp;jobFamilyGroup=b0d5a0c394c810a2b2b427813c504821</t>
+  </si>
+  <si>
+    <t>https://careers.heb.com/digital/jobs?keywords=software</t>
+  </si>
+  <si>
+    <t>Forethought AI</t>
+  </si>
+  <si>
+    <t>https://forethought.ai/careers#open-positions</t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t>https://careers.amd.com/careers-home/jobs?keywords=Software&amp;sortBy=relevance&amp;page=1&amp;country=United%20States&amp;tags1=Yes</t>
+  </si>
+  <si>
+    <t>Nvidia</t>
+  </si>
+  <si>
+    <t>https://nvidia.wd5.myworkdayjobs.com/NVIDIAExternalCareerSite?locationHierarchy2=0c3f5f117e9a0101f6422f0fe79d0000&amp;locationHierarchy2=0c3f5f117e9a0101f63dc469c3010000&amp;locationHierarchy1=2fcb99c455831013ea52fb338f2932d8&amp;timeType=5509c0b5959810ac0029943377d47364&amp;jobFamilyGroup=0c40f6bd1d8f10ae43ffbd1459047e84&amp;jobFamilyGroup=0c40f6bd1d8f10ae43ffb5dd06f47e7e&amp;jobFamilyGroup=0c40f6bd1d8f10ae43ffda1e8d447e94</t>
+  </si>
+  <si>
+    <t>Intel</t>
+  </si>
+  <si>
+    <t>https://intel.wd1.myworkdayjobs.com/External?locations=1e4a4eb3adf101b8aec18a77bf810dd0&amp;locations=1e4a4eb3adf1018c4bf78f77bf8112d0&amp;locations=1e4a4eb3adf10129d05fe377bf815dd0&amp;locations=1e4a4eb3adf1019ec42cde77bf8158d0&amp;locations=1e4a4eb3adf10118b1dfe877bf8162d0&amp;locations=9225dd5a24931001586f2d984f1e0000&amp;locations=da6b8032b879100204a63a809f6c0000&amp;locations=1e4a4eb3adf10146fd5c5276bf81eece&amp;locations=1e4a4eb3adf1011246675c76bf81f8ce&amp;locations=1e4a4eb3adf1016541777876bf8111cf&amp;locations=1e4a4eb3adf101fa2a777d76bf8116cf&amp;timeType=dc193d6170de10860883d9bf7c0e01a9&amp;jobFamilyGroup=dc8bf79476611087d67b2cccdde47034&amp;jobFamilyGroup=dc8bf79476611087d67aed516c5e702c</t>
+  </si>
+  <si>
+    <t>Microchip</t>
+  </si>
+  <si>
+    <t>https://wd5.myworkdaysite.com/en-US/recruiting/microchiphr/External?q=Software&amp;locationCountry=bc33aa3152ec42d4995f4791a106ed09&amp;timeType=51c161e7620310f46a28a73d306c1426&amp;timeType=51c161e7620310f46a28a73b731c1425&amp;zz_LRV_Job_Category_Requisition_Extended=57f4a35d19da01fdd79c79636501c399</t>
+  </si>
+  <si>
+    <t>Qualcomm</t>
+  </si>
+  <si>
+    <t>https://careers.qualcomm.com/careers?query=Software&amp;location=USA&amp;skill=Python&amp;skill=Debugging&amp;skill=Linux&amp;skill=Computer%20Science&amp;skill=Git&amp;skill=Coding&amp;skill=Java&amp;skill=Machine%20Learning&amp;skill=Software%20Engineering&amp;skill=Scripting&amp;skill=Testing&amp;skill=Docker&amp;seniority=Entry&amp;pid=446705678758&amp;domain=qualcomm.com&amp;sort_by=relevance</t>
+  </si>
+  <si>
+    <t>Synopsis</t>
+  </si>
+  <si>
+    <t>https://careers.synopsys.com/search-jobs/Software/44408/1</t>
+  </si>
+  <si>
+    <t>Dwave</t>
+  </si>
+  <si>
+    <t>https://ats.rippling.com/d-wave-quantum/jobs?searchQuery=Software&amp;workplaceType=&amp;country=&amp;state=&amp;city=&amp;page=0</t>
+  </si>
+  <si>
+    <t>Coreview</t>
+  </si>
+  <si>
+    <t>https://coreview.careers.hibob.com/jobs?department=Development</t>
+  </si>
+  <si>
+    <t>Paypal</t>
+  </si>
+  <si>
+    <t>https://paypal.eightfold.ai/careers?query=Software&amp;start=0&amp;location=Dripping+Springs%2C+Texas%2C+US&amp;pid=274907520442&amp;sort_by=solr&amp;filter_distance=80&amp;filter_include_remote=1&amp;filter_job_category=Software+Engineering</t>
+  </si>
+  <si>
+    <t>MongoDB</t>
+  </si>
+  <si>
+    <t>https://www.mongodb.com/company/careers/teams/engineering</t>
+  </si>
+  <si>
+    <t>Affirm</t>
+  </si>
+  <si>
+    <t>https://www.affirm.com/careers</t>
+  </si>
+  <si>
+    <t>Arm</t>
+  </si>
+  <si>
+    <t>https://careers.arm.com/search-jobs/Software?orgIds=33099&amp;kt=1</t>
+  </si>
+  <si>
+    <t>Geico</t>
+  </si>
+  <si>
+    <t>http://geico.wd1.myworkdayjobs.com/External?q=Software</t>
   </si>
 </sst>
 </file>
@@ -484,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,23 +921,288 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
         <v>40</v>
       </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>119</v>
+      </c>
+      <c r="B39" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>121</v>
+      </c>
+      <c r="B40" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>123</v>
+      </c>
+      <c r="B41" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>125</v>
+      </c>
+      <c r="B42" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>127</v>
+      </c>
+      <c r="B43" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>129</v>
+      </c>
+      <c r="B44" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>131</v>
+      </c>
+      <c r="B45" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>133</v>
+      </c>
+      <c r="B46" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>135</v>
+      </c>
+      <c r="B47" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>137</v>
+      </c>
+      <c r="B48" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>139</v>
+      </c>
+      <c r="B49" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>141</v>
+      </c>
+      <c r="B50" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B16" r:id="rId1" xr:uid="{1C4284C0-DF9B-44C9-9FD9-E8D34C386E04}"/>
+    <hyperlink ref="B20" r:id="rId2" xr:uid="{09B6F7E7-8163-413A-8F45-79FA415489A2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -642,10 +1210,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AB1A93-6E1B-431E-965F-8630E7677FC9}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A14" sqref="A14:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,6 +1238,107 @@
         <v>22</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -677,10 +1346,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B70231-856F-450B-820E-DB07789D80FB}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,13 +1360,32 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s">
         <v>36</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{44E04C79-6C4E-457C-B1AE-46D478F1A60F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -719,15 +1407,43 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FBC180A-DB53-4F4E-B78F-B3414A0B4774}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="109.7109375" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -736,7 +1452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3716E9E3-09CF-4B44-8270-01142D288346}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>